<commit_message>
gui button click generates po template
</commit_message>
<xml_diff>
--- a/po_template.xlsx
+++ b/po_template.xlsx
@@ -46,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -354,12 +357,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Hong Infinity Insulated Glass</t>
+          <t>Hong Infinity Insulated Glass Inc.</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Purchase Order</t>
         </is>

</xml_diff>